<commit_message>
Updated Roster and Added Notes for Geography
</commit_message>
<xml_diff>
--- a/Roster.xlsx
+++ b/Roster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\Github\Beethoven-Class-IX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B90F9A2-D592-46FE-AC2B-DA5D7F7355CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB68455-526E-4D78-87DB-4481415C99A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,7 +556,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +575,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,7 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,6 +800,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1370,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,7 +1496,7 @@
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="12"/>
@@ -1573,7 +1584,7 @@
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="12"/>

</xml_diff>

<commit_message>
Update Roster dan Kisi2 Taekwondo
</commit_message>
<xml_diff>
--- a/Roster.xlsx
+++ b/Roster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\GitHub\Beethoven-Class-IX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repositories\Beethoven-Class-IX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E647AD39-DB40-4F59-B14D-6DF67540BD27}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307B7D5E-1F5B-47BF-91AC-6FBAE2DABF72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,29 +856,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -959,6 +936,29 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -1165,17 +1165,17 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RABU" dataDxfId="10"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="KAMIS" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="JUMAT" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{676E886E-C19B-4634-8612-D3DAEC7983F5}" name="#" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{676E886E-C19B-4634-8612-D3DAEC7983F5}" name="#" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:B8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:B8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="HARI" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="CATATAN" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="HARI" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="CATATAN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1450,7 +1450,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,8 +1541,8 @@
       <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>34</v>
@@ -1565,7 +1565,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>34</v>
@@ -1647,7 +1647,7 @@
         <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="1">
@@ -1667,8 +1667,8 @@
       <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="1">

</xml_diff>